<commit_message>
dictionnaire de données EN
modification en anglais
</commit_message>
<xml_diff>
--- a/Base de données (à compléter)/Dictionnaire de données.xlsx
+++ b/Base de données (à compléter)/Dictionnaire de données.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robar\Desktop\CAMPUS CONTEST 2\BDD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robar\Desktop\CAMPUS CONTEST 2\Manga-\Base de données (à compléter)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6700D0E3-2C54-44C3-A20B-AE7E24BCF17F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F15A99-FAC9-41E8-8D1A-9D4CD6CB35BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="93">
   <si>
     <t>TABLE</t>
   </si>
@@ -59,9 +59,6 @@
     <t>identifiant unique du client</t>
   </si>
   <si>
-    <t>Nom</t>
-  </si>
-  <si>
     <t>VARCHAR(255)</t>
   </si>
   <si>
@@ -71,30 +68,18 @@
     <t>nom du client</t>
   </si>
   <si>
-    <t>prénom</t>
-  </si>
-  <si>
     <t>prénom du client</t>
   </si>
   <si>
-    <t>téléphone</t>
-  </si>
-  <si>
     <t>NULL</t>
   </si>
   <si>
     <t>téléphone du client, peut être NULL si le mail est renseigné</t>
   </si>
   <si>
-    <t>E-mail</t>
-  </si>
-  <si>
     <t>mail du client, peut être NULL si le téléphone est renseigné</t>
   </si>
   <si>
-    <t>adresse_id</t>
-  </si>
-  <si>
     <t>INT(11)</t>
   </si>
   <si>
@@ -104,9 +89,6 @@
     <t>Lien vers la ligne de la table adresse du client</t>
   </si>
   <si>
-    <t>Adresse</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -116,102 +98,57 @@
     <t>Identifiant de la ligne de l'adresse</t>
   </si>
   <si>
-    <t>numéro</t>
-  </si>
-  <si>
     <t>INT(4)</t>
   </si>
   <si>
     <t>numéro de la rue</t>
   </si>
   <si>
-    <t>rue</t>
-  </si>
-  <si>
     <t>nom de la rue</t>
   </si>
   <si>
-    <t>code_postal</t>
-  </si>
-  <si>
     <t>code postal</t>
   </si>
   <si>
-    <t>ville</t>
-  </si>
-  <si>
     <t>nom de la ville</t>
   </si>
   <si>
-    <t>pays</t>
-  </si>
-  <si>
     <t>nom du pays</t>
   </si>
   <si>
-    <t>Location</t>
-  </si>
-  <si>
     <t>Identifiant unique d'une location</t>
   </si>
   <si>
-    <t>date_début</t>
-  </si>
-  <si>
     <t>DATE</t>
   </si>
   <si>
     <t>date du début de la location</t>
   </si>
   <si>
-    <t>date_fin</t>
-  </si>
-  <si>
     <t>date de fin de la location</t>
   </si>
   <si>
-    <t>retourné</t>
-  </si>
-  <si>
     <t>BOOL</t>
   </si>
   <si>
     <t>est-ce que le livre à été rendu (Oui / Non)</t>
   </si>
   <si>
-    <t>disponible</t>
-  </si>
-  <si>
-    <t>Auteur</t>
-  </si>
-  <si>
     <t>Identifiant unique d'un auteur</t>
   </si>
   <si>
-    <t>nom</t>
-  </si>
-  <si>
     <t>nom de l'auteur</t>
   </si>
   <si>
     <t>prénom de l'auteur</t>
   </si>
   <si>
-    <t>année_de_naissance</t>
-  </si>
-  <si>
     <t>année de naissance de l'auteur</t>
   </si>
   <si>
-    <t>nationalité</t>
-  </si>
-  <si>
     <t>nationalité de l'auteur</t>
   </si>
   <si>
-    <t>Livre</t>
-  </si>
-  <si>
     <t>Identifiant unique d'un livre</t>
   </si>
   <si>
@@ -221,60 +158,30 @@
     <t>numéro ISBN correspondant au livre</t>
   </si>
   <si>
-    <t>titre</t>
-  </si>
-  <si>
     <t>titre du livre</t>
   </si>
   <si>
-    <t>date_publication</t>
-  </si>
-  <si>
     <t>date de publication du livre</t>
   </si>
   <si>
-    <t>nombre_de_page</t>
-  </si>
-  <si>
     <t>INT(5)</t>
   </si>
   <si>
     <t>nombre de page du livre</t>
   </si>
   <si>
-    <t>date_acquisition</t>
-  </si>
-  <si>
     <t>date d'acquisition du livre par la librairie</t>
   </si>
   <si>
-    <t>langue</t>
-  </si>
-  <si>
     <t>langue du livre</t>
   </si>
   <si>
-    <t>auteur_id</t>
-  </si>
-  <si>
     <t>type_id</t>
   </si>
   <si>
-    <t>location_id</t>
-  </si>
-  <si>
-    <t>exemplaire_id</t>
-  </si>
-  <si>
-    <t>Exemplaire</t>
-  </si>
-  <si>
     <t>Identifiant unique de l'exemplaire correspondant au livre</t>
   </si>
   <si>
-    <t>numéro_exemplaire</t>
-  </si>
-  <si>
     <t>numéro d'exemplaire d'un livre</t>
   </si>
   <si>
@@ -284,9 +191,6 @@
     <t>Identifiant unique du type de livre</t>
   </si>
   <si>
-    <t>nom_du_type</t>
-  </si>
-  <si>
     <t>nom du type de livre (manga, BD ou autre)</t>
   </si>
   <si>
@@ -308,10 +212,103 @@
     <t xml:space="preserve">complément optionnel </t>
   </si>
   <si>
-    <t>complément</t>
-  </si>
-  <si>
     <t>Client</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>e-mail</t>
+  </si>
+  <si>
+    <t>adress_id</t>
+  </si>
+  <si>
+    <t>renting_id</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>street</t>
+  </si>
+  <si>
+    <t>postal_code</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>complement</t>
+  </si>
+  <si>
+    <t>start_date</t>
+  </si>
+  <si>
+    <t>end_date</t>
+  </si>
+  <si>
+    <t>return</t>
+  </si>
+  <si>
+    <t>availability</t>
+  </si>
+  <si>
+    <t>date_of_birth</t>
+  </si>
+  <si>
+    <t>nationality</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>publication_date</t>
+  </si>
+  <si>
+    <t>number_of_page</t>
+  </si>
+  <si>
+    <t>purchase_date</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>author_id</t>
+  </si>
+  <si>
+    <t>copy_id</t>
+  </si>
+  <si>
+    <t>copy_number</t>
+  </si>
+  <si>
+    <t>type_name</t>
+  </si>
+  <si>
+    <t>Copy</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Renting</t>
+  </si>
+  <si>
+    <t>Adress</t>
+  </si>
+  <si>
+    <t>Book</t>
   </si>
 </sst>
 </file>
@@ -798,8 +795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A8"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -828,7 +825,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>93</v>
+        <v>60</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -846,91 +843,91 @@
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
       <c r="B7" s="2" t="s">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
       <c r="B8" s="2" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -966,109 +963,109 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
-        <v>24</v>
+        <v>91</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="12"/>
       <c r="B13" s="2" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
       <c r="B14" s="2" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="12"/>
       <c r="B15" s="2" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="12"/>
       <c r="B16" s="2" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="12"/>
       <c r="B17" s="2" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="13"/>
       <c r="B18" s="2" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>91</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1104,79 +1101,79 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
-        <v>39</v>
+        <v>90</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="10"/>
       <c r="B23" s="2" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
       <c r="B24" s="2" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="10"/>
       <c r="B25" s="2" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="10"/>
       <c r="B26" s="2" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1212,79 +1209,79 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
-        <v>50</v>
+        <v>89</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="12"/>
       <c r="B31" s="2" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="12"/>
       <c r="B32" s="2" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="12"/>
       <c r="B33" s="2" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="13"/>
       <c r="B34" s="2" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1320,169 +1317,169 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
-        <v>59</v>
+        <v>92</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="12"/>
       <c r="B39" s="2" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="12"/>
       <c r="B40" s="2" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="12"/>
       <c r="B41" s="2" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="12"/>
       <c r="B42" s="2" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="12"/>
       <c r="B43" s="2" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="12"/>
       <c r="B44" s="2" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="12"/>
       <c r="B45" s="2" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="12"/>
       <c r="B46" s="2" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>88</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="12"/>
       <c r="B47" s="2" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="13"/>
       <c r="B48" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>90</v>
+        <v>58</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1518,34 +1515,34 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="11" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="13"/>
       <c r="B53" s="2" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -1581,34 +1578,34 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="11" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="13"/>
       <c r="B58" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -1627,13 +1624,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A57:A58"/>
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="A12:A18"/>
     <mergeCell ref="A22:A26"/>
     <mergeCell ref="A30:A34"/>
     <mergeCell ref="A38:A48"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A57:A58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>